<commit_message>
Added Gantt_diagramV2.png and changed Gantt_diagram.xlsx
</commit_message>
<xml_diff>
--- a/diagrams/Gantt_diagram.xlsx
+++ b/diagrams/Gantt_diagram.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\EFREI\Semestre5 MOBILITE\Advanced WEB programming\PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roland\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F240132F-5C27-4FF4-8A9D-F4C8694F5E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B209C1F-B537-4266-A1DE-52598EE8EC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7AA6A491-8344-488B-B4F6-CD981A99F086}"/>
   </bookViews>
@@ -65,21 +65,9 @@
     <t>Start Graphic Chart/Logo...</t>
   </si>
   <si>
-    <t>Table structure diagram</t>
-  </si>
-  <si>
-    <t>Adding Diagrams (ER+Structure)</t>
-  </si>
-  <si>
     <t>Setup Github</t>
   </si>
   <si>
-    <t xml:space="preserve">Use Case Diagram + Gantt </t>
-  </si>
-  <si>
-    <t>.vue files + Use case Diagram</t>
-  </si>
-  <si>
     <t>improve .vue/clearer pages</t>
   </si>
   <si>
@@ -107,9 +95,6 @@
     <t>Implements UI</t>
   </si>
   <si>
-    <t>Implements New Fonctionalities(Log in...)</t>
-  </si>
-  <si>
     <t>Bug Fixes</t>
   </si>
   <si>
@@ -141,6 +126,21 @@
   </si>
   <si>
     <t>Sep 15-21</t>
+  </si>
+  <si>
+    <t>Setup SERVER</t>
+  </si>
+  <si>
+    <t>BOTH</t>
+  </si>
+  <si>
+    <t>Start Front-end with tables</t>
+  </si>
+  <si>
+    <t>Implement Log In</t>
+  </si>
+  <si>
+    <t>Link Log IN to DB</t>
   </si>
 </sst>
 </file>
@@ -162,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +187,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -200,15 +206,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -220,6 +220,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +577,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,66 +596,66 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>21</v>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -677,10 +697,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -693,15 +713,11 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -714,13 +730,13 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="E7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="5"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -732,12 +748,11 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="5"/>
+      <c r="F8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="6"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
@@ -749,13 +764,10 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="H9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -766,13 +778,13 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="H10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -785,7 +797,9 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -798,12 +812,14 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -818,7 +834,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -832,6 +848,9 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -908,11 +927,9 @@
       <c r="K20" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>